<commit_message>
fix(influxdb): influxdb/kafka data dir choose #125
influxdb data dir choose fix
</commit_message>
<xml_diff>
--- a/dbm-ui/backend/ticket/exclusive_ticket.xlsx
+++ b/dbm-ui/backend/ticket/exclusive_ticket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaomugong/Works/tencent/dbs/blueking-dbm/dbm-ui/backend/ticket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3058872-0741-2248-9824-8375B9399247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA895D-2D7A-054C-9A28-EA7A86C3F8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_mysql_exclusive" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,14 @@
     <sheet name="cluster_kafka_exclusive" sheetId="3" r:id="rId3"/>
     <sheet name="cluster_hdfs_exclusive" sheetId="4" r:id="rId4"/>
     <sheet name="cluster_es_exclusive" sheetId="5" r:id="rId5"/>
-    <sheet name="cluster_influxdb_exclusive" sheetId="6" r:id="rId6"/>
-    <sheet name="cluster_pulsar_exclusive" sheetId="7" r:id="rId7"/>
+    <sheet name="cluster_pulsar_exclusive" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="53">
   <si>
     <t>能否并行</t>
   </si>
@@ -223,28 +222,6 @@
   </si>
   <si>
     <t>Pulsar 集群删除</t>
-  </si>
-  <si>
-    <t>InfluxDB 集群停用</t>
-  </si>
-  <si>
-    <t>InfluxDB 集群删除</t>
-  </si>
-  <si>
-    <t>InfluxDB 集群重启</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>InfluxDB 实例替换</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>InfluxDB 集群删除</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>InfluxDB 集群启用</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6397,11 +6374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F0BDC2-B2A8-6A48-AC30-E64A5C66E762}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51380A97-C090-4345-BAF7-755EB452DCA3}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6411,142 +6388,6 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="33" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="33" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="33" thickBot="1">
-      <c r="A4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="33" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="33" thickBot="1">
-      <c r="A6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51380A97-C090-4345-BAF7-755EB452DCA3}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:6" ht="33" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="2" t="s">

</xml_diff>

<commit_message>
fix(redis): 工具箱任务互斥定义 close #874
</commit_message>
<xml_diff>
--- a/dbm-ui/backend/ticket/exclusive_ticket.xlsx
+++ b/dbm-ui/backend/ticket/exclusive_ticket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaomugong/Works/tencent/dbs/blueking-dbm/dbm-ui/backend/ticket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA895D-2D7A-054C-9A28-EA7A86C3F8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E579F-A5AE-1347-B7EF-C7C072E9F53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1280" yWindow="-21100" windowWidth="30240" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_mysql_exclusive" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="68">
   <si>
     <t>能否并行</t>
   </si>
@@ -64,28 +64,6 @@
   </si>
   <si>
     <t>主从互换</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>替换</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF333333"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>Proxy</t>
-    </r>
   </si>
   <si>
     <r>
@@ -222,6 +200,75 @@
   </si>
   <si>
     <t>Pulsar 集群删除</t>
+  </si>
+  <si>
+    <t>变更SQL执行</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>替换</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proxy</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB实例权限克隆</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>集群容量变更</t>
+  </si>
+  <si>
+    <t>Proxy缩容</t>
+  </si>
+  <si>
+    <t>Proxy扩容</t>
+  </si>
+  <si>
+    <t>整机替换</t>
+  </si>
+  <si>
+    <t>主从故障切换</t>
+  </si>
+  <si>
+    <t>数据构造记录删除</t>
+  </si>
+  <si>
+    <t>数据校验与修复</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>集群分片数变更</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>集群数据复制</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>集群类型变更</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>集群数据构造</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增slave节点</t>
+  </si>
+  <si>
+    <t>构造实例数据回写</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -665,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S201"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="15"/>
@@ -679,7 +726,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -700,7 +747,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
@@ -715,22 +762,22 @@
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="36.75" customHeight="1">
@@ -738,58 +785,58 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="36.75" customHeight="1">
@@ -797,58 +844,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="36.75" customHeight="1">
@@ -856,58 +903,58 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="N4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="36.75" customHeight="1">
@@ -915,58 +962,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="36.75" customHeight="1">
@@ -974,58 +1021,58 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36.75" customHeight="1">
@@ -1033,58 +1080,58 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="N7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36.75" customHeight="1">
@@ -1092,58 +1139,58 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="36.75" customHeight="1">
@@ -1151,58 +1198,58 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="36.75" customHeight="1">
@@ -1210,58 +1257,58 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="36.75" customHeight="1">
@@ -1269,58 +1316,58 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="36.75" customHeight="1">
@@ -1328,58 +1375,58 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="36.75" customHeight="1">
@@ -1387,412 +1434,412 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="36.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="36.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="36.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="36.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="36.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="36.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="16">
@@ -5625,335 +5672,1653 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.6640625" customWidth="1"/>
+    <col min="17" max="22" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32">
+    <row r="1" spans="1:23" ht="33" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="32">
+      <c r="K1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="33" thickBot="1">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="33" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="32">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="33" thickBot="1">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="32">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="33" thickBot="1">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="32">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="33" thickBot="1">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="32">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="33" thickBot="1">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="32">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="33" thickBot="1">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="32">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="33" thickBot="1">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="32">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="33" thickBot="1">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="32">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="33" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="27" customHeight="1" thickBot="1">
+      <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="32" customHeight="1" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="36" customHeight="1" thickBot="1">
+      <c r="A14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="33" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="33" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="33" thickBot="1">
+      <c r="A17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="33" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="33" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="33" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="33" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="33" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="33" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="W23" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -5980,119 +7345,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="36.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -6116,119 +7481,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -6252,119 +7617,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32">
       <c r="A5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -6377,7 +7742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51380A97-C090-4345-BAF7-755EB452DCA3}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -6388,119 +7753,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="33" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" thickBot="1">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "fix(redis): 修复Redis生命周期统计程序  (#1130)"
This reverts commit b4f62b99e266c02456e0afbecabc39807782d866.
</commit_message>
<xml_diff>
--- a/dbm-ui/backend/ticket/exclusive_ticket.xlsx
+++ b/dbm-ui/backend/ticket/exclusive_ticket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaomugong/Works/tencent/dbs/blueking-dbm/dbm-ui/backend/ticket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A1001E-9BEC-4D45-AA63-AA5CA63C2765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA895D-2D7A-054C-9A28-EA7A86C3F8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1280" yWindow="-21100" windowWidth="30240" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_mysql_exclusive" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="53">
   <si>
     <t>能否并行</t>
   </si>
@@ -64,6 +64,28 @@
   </si>
   <si>
     <t>主从互换</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>替换</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proxy</t>
+    </r>
   </si>
   <si>
     <r>
@@ -119,6 +141,9 @@
   </si>
   <si>
     <t>Redis 集群禁用</t>
+  </si>
+  <si>
+    <t>Proxy 扩缩容</t>
   </si>
   <si>
     <t>Redis 扩缩容</t>
@@ -198,75 +223,12 @@
   <si>
     <t>Pulsar 集群删除</t>
   </si>
-  <si>
-    <t>变更SQL执行</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>替换</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF333333"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>Proxy</t>
-    </r>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB实例权限克隆</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>集群容量变更</t>
-  </si>
-  <si>
-    <t>Proxy缩容</t>
-  </si>
-  <si>
-    <t>Proxy扩容</t>
-  </si>
-  <si>
-    <t>整机替换</t>
-  </si>
-  <si>
-    <t>主从故障切换</t>
-  </si>
-  <si>
-    <t>数据构造记录删除</t>
-  </si>
-  <si>
-    <t>新增slave节点</t>
-  </si>
-  <si>
-    <t>集群分片数变更</t>
-  </si>
-  <si>
-    <t>集群类型变更</t>
-  </si>
-  <si>
-    <t>集群数据构造</t>
-  </si>
-  <si>
-    <t>集群数据复制</t>
-  </si>
-  <si>
-    <t>构造实例数据回写</t>
-  </si>
-  <si>
-    <t>数据校验与修复</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -332,28 +294,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="SimSun"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -369,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -416,52 +356,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -486,24 +387,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -782,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.6640625" defaultRowHeight="15"/>
@@ -796,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -817,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
@@ -832,22 +715,22 @@
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="36.75" customHeight="1">
@@ -855,58 +738,58 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="36.75" customHeight="1">
@@ -914,58 +797,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="36.75" customHeight="1">
@@ -973,58 +856,58 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="36.75" customHeight="1">
@@ -1032,58 +915,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="36.75" customHeight="1">
@@ -1091,58 +974,58 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="36.75" customHeight="1">
@@ -1150,58 +1033,58 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="36.75" customHeight="1">
@@ -1209,58 +1092,58 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="36.75" customHeight="1">
@@ -1268,58 +1151,58 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="36.75" customHeight="1">
@@ -1327,58 +1210,58 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="36.75" customHeight="1">
@@ -1386,58 +1269,58 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="36.75" customHeight="1">
@@ -1445,58 +1328,58 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="36.75" customHeight="1">
@@ -1504,412 +1387,412 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="36.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="36.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="36.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="36.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="36.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="36.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="16">
@@ -5742,1516 +5625,335 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="21" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="33" thickBot="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="32">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" ht="33" thickBot="1">
-      <c r="A2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="33" thickBot="1">
-      <c r="A3" s="11" t="s">
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="32">
+      <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="33" thickBot="1">
-      <c r="A4" s="11" t="s">
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="32">
+      <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V4" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="33" thickBot="1">
-      <c r="A5" s="11" t="s">
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="32">
+      <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V5" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="33" thickBot="1">
-      <c r="A6" s="11" t="s">
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32">
+      <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="33" thickBot="1">
-      <c r="A7" s="11" t="s">
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="32">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V7" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="33" thickBot="1">
-      <c r="A8" s="11" t="s">
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="32">
+      <c r="A7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="33" thickBot="1">
-      <c r="A9" s="11" t="s">
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="32">
+      <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V9" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="33" thickBot="1">
-      <c r="A10" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V10" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="27" customHeight="1" thickBot="1">
-      <c r="A11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U11" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V11" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="32" customHeight="1" thickBot="1">
-      <c r="A12" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T12" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V12" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="36" customHeight="1" thickBot="1">
-      <c r="A13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V13" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="33" thickBot="1">
-      <c r="A14" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="O14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="U14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V14" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="33" thickBot="1">
-      <c r="A15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U15" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V15" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="33" thickBot="1">
-      <c r="A16" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S16" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="U16" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V16" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" ht="33" thickBot="1">
-      <c r="A17" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="33" thickBot="1">
-      <c r="A18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R18" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="S18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V18" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="33" thickBot="1">
-      <c r="A19" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S19" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="T19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" ht="33" thickBot="1">
-      <c r="A20" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="S20" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="T20" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="U20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="V20" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="33" thickBot="1">
-      <c r="A21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="P21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="R21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="S21" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="T21" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="U21" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="V21" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" ht="33" thickBot="1">
-      <c r="A22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="S22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="U22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V22" s="14" t="s">
-        <v>18</v>
+      <c r="B8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="32">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="32">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -7278,119 +5980,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="36.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7414,119 +6116,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7550,119 +6252,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32">
       <c r="A4" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32">
       <c r="A5" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7675,7 +6377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51380A97-C090-4345-BAF7-755EB452DCA3}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -7686,119 +6388,119 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="33" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" thickBot="1">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" thickBot="1">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" thickBot="1">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(backend): sqlserver单据互斥回退 #6363 # Reviewed, transaction id: 15973
</commit_message>
<xml_diff>
--- a/dbm-ui/backend/ticket/exclusive_ticket.xlsx
+++ b/dbm-ui/backend/ticket/exclusive_ticket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\blueking-dbm\dbm-ui\backend\ticket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98F2C0A-E671-4125-AF46-4AFE783BEC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF29B5-918D-4E45-BED3-505028009B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57945" yWindow="435" windowWidth="26175" windowHeight="13155" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58650" yWindow="2055" windowWidth="26175" windowHeight="14985" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_mysql_exclusive" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="101">
   <si>
     <t>能否并行</t>
   </si>
@@ -352,6 +352,14 @@
   <si>
     <t>SQLServer 集群授权</t>
     <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQLServer 集群禁用</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6153,7 +6161,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.15"/>
@@ -8083,7 +8091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -9504,15 +9512,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3040E7F9-8649-42DD-BAEB-BE90D023AAB5}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="45.45" thickBot="1">
+    <row r="1" spans="1:14" ht="45.45" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -9552,8 +9560,11 @@
       <c r="M1" s="28" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N1" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="45.45" thickBot="1">
       <c r="A2" s="28" t="s">
         <v>87</v>
       </c>
@@ -9593,8 +9604,11 @@
       <c r="M2" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N2" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45.45" thickBot="1">
       <c r="A3" s="28" t="s">
         <v>88</v>
       </c>
@@ -9634,8 +9648,11 @@
       <c r="M3" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N3" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="45.45" thickBot="1">
       <c r="A4" s="28" t="s">
         <v>89</v>
       </c>
@@ -9675,8 +9692,11 @@
       <c r="M4" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N4" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="45.45" thickBot="1">
       <c r="A5" s="28" t="s">
         <v>90</v>
       </c>
@@ -9716,8 +9736,11 @@
       <c r="M5" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N5" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="45.45" thickBot="1">
       <c r="A6" s="28" t="s">
         <v>91</v>
       </c>
@@ -9757,8 +9780,11 @@
       <c r="M6" s="30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N6" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="45.45" thickBot="1">
       <c r="A7" s="28" t="s">
         <v>92</v>
       </c>
@@ -9798,8 +9824,11 @@
       <c r="M7" s="30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N7" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="45.45" thickBot="1">
       <c r="A8" s="28" t="s">
         <v>93</v>
       </c>
@@ -9839,8 +9868,11 @@
       <c r="M8" s="30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N8" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45.45" thickBot="1">
       <c r="A9" s="28" t="s">
         <v>94</v>
       </c>
@@ -9880,8 +9912,11 @@
       <c r="M9" s="30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N9" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="45.45" thickBot="1">
       <c r="A10" s="28" t="s">
         <v>95</v>
       </c>
@@ -9921,8 +9956,11 @@
       <c r="M10" s="30" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N10" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="45.45" thickBot="1">
       <c r="A11" s="28" t="s">
         <v>96</v>
       </c>
@@ -9962,8 +10000,11 @@
       <c r="M11" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="30.45" thickBot="1">
+      <c r="N11" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="30.45" thickBot="1">
       <c r="A12" s="28" t="s">
         <v>97</v>
       </c>
@@ -10003,8 +10044,11 @@
       <c r="M12" s="30" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="45.45" thickBot="1">
+      <c r="N12" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45.45" thickBot="1">
       <c r="A13" s="28" t="s">
         <v>98</v>
       </c>
@@ -10043,6 +10087,53 @@
       </c>
       <c r="M13" s="29" t="s">
         <v>19</v>
+      </c>
+      <c r="N13" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="45.45" thickBot="1">
+      <c r="A14" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(backend): sqlserver数据迁移分类全备和增量 #6428 # Reviewed, transaction id: 16387
</commit_message>
<xml_diff>
--- a/dbm-ui/backend/ticket/exclusive_ticket.xlsx
+++ b/dbm-ui/backend/ticket/exclusive_ticket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProject\blueking-dbm\dbm-ui\backend\ticket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AF29B5-918D-4E45-BED3-505028009B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA99C27-32BC-45BB-BF3F-372375B360E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58650" yWindow="2055" windowWidth="26175" windowHeight="14985" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cluster_mysql_exclusive" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="102">
   <si>
     <t>能否并行</t>
   </si>
@@ -342,10 +342,6 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>SQLServer 数据迁移</t>
-    <phoneticPr fontId="14" type="noConversion"/>
-  </si>
-  <si>
     <t>SQLServer 清档</t>
     <phoneticPr fontId="14" type="noConversion"/>
   </si>
@@ -360,6 +356,14 @@
   <si>
     <t>N</t>
     <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQLServer 全备迁移</t>
+    <phoneticPr fontId="14" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQLServer 增量迁移</t>
+    <phoneticPr fontId="14" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -757,7 +761,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -904,6 +908,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9512,15 +9519,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3040E7F9-8649-42DD-BAEB-BE90D023AAB5}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="45.45" thickBot="1">
+    <row r="1" spans="1:15" ht="45.45" thickBot="1">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -9552,19 +9559,22 @@
         <v>95</v>
       </c>
       <c r="K1" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N1" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="45.45" thickBot="1">
+    </row>
+    <row r="2" spans="1:15" ht="45.45" thickBot="1">
       <c r="A2" s="28" t="s">
         <v>87</v>
       </c>
@@ -9602,13 +9612,16 @@
         <v>85</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="N2" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="45.45" thickBot="1">
+        <v>19</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="45.45" thickBot="1">
       <c r="A3" s="28" t="s">
         <v>88</v>
       </c>
@@ -9646,13 +9659,16 @@
         <v>85</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="N3" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="45.45" thickBot="1">
+        <v>19</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="45.45" thickBot="1">
       <c r="A4" s="28" t="s">
         <v>89</v>
       </c>
@@ -9690,13 +9706,16 @@
         <v>85</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="N4" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45.45" thickBot="1">
+        <v>19</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45.45" thickBot="1">
       <c r="A5" s="28" t="s">
         <v>90</v>
       </c>
@@ -9737,10 +9756,13 @@
         <v>19</v>
       </c>
       <c r="N5" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="45.45" thickBot="1">
+        <v>19</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="45.45" thickBot="1">
       <c r="A6" s="28" t="s">
         <v>91</v>
       </c>
@@ -9778,13 +9800,16 @@
         <v>19</v>
       </c>
       <c r="M6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="N6" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="45.45" thickBot="1">
+      <c r="O6" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="45.45" thickBot="1">
       <c r="A7" s="28" t="s">
         <v>92</v>
       </c>
@@ -9822,13 +9847,16 @@
         <v>19</v>
       </c>
       <c r="M7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="N7" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="45.45" thickBot="1">
+      <c r="O7" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="45.45" thickBot="1">
       <c r="A8" s="28" t="s">
         <v>93</v>
       </c>
@@ -9866,13 +9894,16 @@
         <v>19</v>
       </c>
       <c r="M8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="N8" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="45.45" thickBot="1">
+      <c r="O8" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="45.45" thickBot="1">
       <c r="A9" s="28" t="s">
         <v>94</v>
       </c>
@@ -9913,10 +9944,13 @@
         <v>85</v>
       </c>
       <c r="N9" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="45.45" thickBot="1">
+        <v>85</v>
+      </c>
+      <c r="O9" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="45.45" thickBot="1">
       <c r="A10" s="28" t="s">
         <v>95</v>
       </c>
@@ -9957,12 +9991,15 @@
         <v>85</v>
       </c>
       <c r="N10" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="45.45" thickBot="1">
+      <c r="A11" s="28" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="45.45" thickBot="1">
-      <c r="A11" s="28" t="s">
-        <v>96</v>
       </c>
       <c r="B11" s="30" t="s">
         <v>86</v>
@@ -9994,146 +10031,205 @@
       <c r="K11" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L11" s="30" t="s">
+      <c r="L11" s="50" t="s">
         <v>85</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="N11" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="30.45" thickBot="1">
+        <v>19</v>
+      </c>
+      <c r="O11" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="45.45" thickBot="1">
       <c r="A12" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30.45" thickBot="1">
+      <c r="A13" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="M13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="N13" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="O13" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="45.45" thickBot="1">
+      <c r="A14" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="45.45" thickBot="1">
-      <c r="A13" s="28" t="s">
+      <c r="B14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45.45" thickBot="1">
+      <c r="A15" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="K13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="L13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="45.45" thickBot="1">
-      <c r="A14" s="28" t="s">
+      <c r="B15" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="L14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="N14" s="29" t="s">
-        <v>100</v>
+      <c r="C15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="N15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="O15" s="29" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>